<commit_message>
paper committed with candidate materials modified
</commit_message>
<xml_diff>
--- a/candidate materials.xlsx
+++ b/candidate materials.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" tabRatio="593" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" tabRatio="593" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="watch Strap" sheetId="1" r:id="rId1"/>
@@ -329,10 +329,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -639,8 +639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F32" sqref="F32:F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -703,26 +703,26 @@
       <c r="A3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="16">
-        <v>3</v>
-      </c>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16">
-        <v>3</v>
-      </c>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16">
-        <v>2</v>
-      </c>
-      <c r="G3" s="16"/>
-      <c r="H3" s="15">
-        <v>2</v>
-      </c>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15">
-        <v>3</v>
-      </c>
-      <c r="K3" s="15"/>
+      <c r="B3" s="15">
+        <v>3</v>
+      </c>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15">
+        <v>3</v>
+      </c>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15">
+        <v>2</v>
+      </c>
+      <c r="G3" s="15"/>
+      <c r="H3" s="16">
+        <v>2</v>
+      </c>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16">
+        <v>3</v>
+      </c>
+      <c r="K3" s="16"/>
     </row>
     <row r="4" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
@@ -749,19 +749,19 @@
         <v>29</v>
       </c>
       <c r="C5">
-        <v>3.4093931837073996</v>
+        <v>3.4089999999999998</v>
       </c>
       <c r="E5">
-        <v>2.26356589147287</v>
+        <v>2.2639999999999998</v>
       </c>
       <c r="G5">
-        <v>2.5272020725388598</v>
+        <v>2.5270000000000001</v>
       </c>
       <c r="I5">
-        <v>2.0696661828737302</v>
+        <v>2.0699999999999998</v>
       </c>
       <c r="K5">
-        <v>2.1603053435114501</v>
+        <v>2.16</v>
       </c>
     </row>
     <row r="6" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -962,23 +962,23 @@
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C13">
         <f>C5/C$11</f>
-        <v>0.68187863674147997</v>
+        <v>0.68179999999999996</v>
       </c>
       <c r="E13">
         <f>E5/E$11</f>
-        <v>0.75452196382429004</v>
+        <v>0.7546666666666666</v>
       </c>
       <c r="G13">
         <f>G5/G$11</f>
-        <v>0.505440414507772</v>
+        <v>0.50540000000000007</v>
       </c>
       <c r="I13">
         <f>I5/I$11</f>
-        <v>0.68988872762457676</v>
+        <v>0.69</v>
       </c>
       <c r="K13">
         <f>K5/K$11</f>
-        <v>0.7201017811704834</v>
+        <v>0.72000000000000008</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
@@ -1183,111 +1183,111 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C20">
-        <f>ABS(C6-C$5)/(MAX(C$5:C$10)-MIN(C$5:C$10))</f>
-        <v>0.46979772790246654</v>
+        <f>ROUND((ABS(C6-C$5)/(MAX(C$5:C$10)-MIN(C$5:C$10))), 4)</f>
+        <v>0.46970000000000001</v>
       </c>
       <c r="E20">
-        <f>ABS(E6-E$5)/(MAX(E$5:E$10)-MIN(E$5:E$10))</f>
-        <v>0.63178294573643501</v>
+        <f>ROUND((ABS(E6-E$5)/(MAX(E$5:E$10)-MIN(E$5:E$10))), 4)</f>
+        <v>0.63200000000000001</v>
       </c>
       <c r="G20">
-        <f>ABS(G6-G$5)/(MAX(G$5:G$10)-MIN(G$5:G$10))</f>
-        <v>0.23639896373057012</v>
+        <f>ROUND((ABS(G6-G$5)/(MAX(G$5:G$10)-MIN(G$5:G$10))), 4)</f>
+        <v>0.23649999999999999</v>
       </c>
       <c r="I20">
-        <f>ABS(I6-I$5)/(MAX(I$5:I$10)-MIN(I$5:I$10))</f>
-        <v>3.4833091436865082E-2</v>
+        <f>ROUND((ABS(I6-I$5)/(MAX(I$5:I$10)-MIN(I$5:I$10))), 4)</f>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="K20">
-        <f>ABS(K6-K$5)/(MAX(K$5:K$10)-MIN(K$5:K$10))</f>
-        <v>0.1381578947368419</v>
+        <f>ROUND((ABS(K6-K$5)/(MAX(K$5:K$10)-MIN(K$5:K$10))), 4)</f>
+        <v>0.13789999999999999</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C21">
-        <f t="shared" ref="C21:E24" si="5">ABS(C7-C$5)/(MAX(C$5:C$10)-MIN(C$5:C$10))</f>
-        <v>0.1364643945691332</v>
+        <f t="shared" ref="C21:C24" si="5">ROUND((ABS(C7-C$5)/(MAX(C$5:C$10)-MIN(C$5:C$10))), 4)</f>
+        <v>0.1363</v>
       </c>
       <c r="E21">
-        <f t="shared" si="5"/>
-        <v>0.13178294573643501</v>
+        <f t="shared" ref="E21:E24" si="6">ROUND((ABS(E7-E$5)/(MAX(E$5:E$10)-MIN(E$5:E$10))), 4)</f>
+        <v>0.13200000000000001</v>
       </c>
       <c r="G21">
-        <f t="shared" ref="G21:G24" si="6">ABS(G7-G$5)/(MAX(G$5:G$10)-MIN(G$5:G$10))</f>
-        <v>0.26360103626942988</v>
+        <f t="shared" ref="G21:G24" si="7">ROUND((ABS(G7-G$5)/(MAX(G$5:G$10)-MIN(G$5:G$10))), 4)</f>
+        <v>0.26350000000000001</v>
       </c>
       <c r="I21">
-        <f t="shared" ref="I21" si="7">ABS(I7-I$5)/(MAX(I$5:I$10)-MIN(I$5:I$10))</f>
-        <v>0.46516690856313492</v>
+        <f t="shared" ref="I21:I24" si="8">ROUND((ABS(I7-I$5)/(MAX(I$5:I$10)-MIN(I$5:I$10))), 4)</f>
+        <v>0.46500000000000002</v>
       </c>
       <c r="K21">
-        <f t="shared" ref="K21" si="8">ABS(K7-K$5)/(MAX(K$5:K$10)-MIN(K$5:K$10))</f>
+        <f t="shared" ref="K21:K24" si="9">ROUND((ABS(K7-K$5)/(MAX(K$5:K$10)-MIN(K$5:K$10))), 4)</f>
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C22">
         <f t="shared" si="5"/>
-        <v>0.53020227209753346</v>
+        <v>0.53029999999999999</v>
       </c>
       <c r="E22">
-        <f t="shared" si="5"/>
-        <v>0.36821705426356499</v>
+        <f t="shared" si="6"/>
+        <v>0.36799999999999999</v>
       </c>
       <c r="G22">
-        <f t="shared" si="6"/>
-        <v>0.23639896373057012</v>
+        <f t="shared" si="7"/>
+        <v>0.23649999999999999</v>
       </c>
       <c r="I22">
-        <f t="shared" ref="I22" si="9">ABS(I8-I$5)/(MAX(I$5:I$10)-MIN(I$5:I$10))</f>
-        <v>0.53483309143686508</v>
+        <f t="shared" si="8"/>
+        <v>0.53500000000000003</v>
       </c>
       <c r="K22">
-        <f t="shared" ref="K22" si="10">ABS(K8-K$5)/(MAX(K$5:K$10)-MIN(K$5:K$10))</f>
-        <v>0.1381578947368419</v>
+        <f t="shared" si="9"/>
+        <v>0.13789999999999999</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C23">
         <f t="shared" si="5"/>
-        <v>0.46979772790246654</v>
+        <v>0.46970000000000001</v>
       </c>
       <c r="E23">
-        <f t="shared" si="5"/>
-        <v>0.36821705426356499</v>
+        <f t="shared" si="6"/>
+        <v>0.36799999999999999</v>
       </c>
       <c r="G23">
-        <f t="shared" si="6"/>
-        <v>0.73639896373057012</v>
+        <f t="shared" si="7"/>
+        <v>0.73650000000000004</v>
       </c>
       <c r="I23">
-        <f t="shared" ref="I23" si="11">ABS(I9-I$5)/(MAX(I$5:I$10)-MIN(I$5:I$10))</f>
-        <v>0.46516690856313492</v>
+        <f t="shared" si="8"/>
+        <v>0.46500000000000002</v>
       </c>
       <c r="K23">
-        <f t="shared" ref="K23" si="12">ABS(K9-K$5)/(MAX(K$5:K$10)-MIN(K$5:K$10))</f>
-        <v>0.1381578947368419</v>
+        <f t="shared" si="9"/>
+        <v>0.13789999999999999</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C24">
         <f t="shared" si="5"/>
-        <v>0.1364643945691332</v>
+        <v>0.1363</v>
       </c>
       <c r="E24">
-        <f t="shared" si="5"/>
-        <v>0.36821705426356499</v>
+        <f t="shared" si="6"/>
+        <v>0.36799999999999999</v>
       </c>
       <c r="G24">
-        <f t="shared" si="6"/>
-        <v>0.23639896373057012</v>
+        <f t="shared" si="7"/>
+        <v>0.23649999999999999</v>
       </c>
       <c r="I24">
-        <f t="shared" ref="I24" si="13">ABS(I10-I$5)/(MAX(I$5:I$10)-MIN(I$5:I$10))</f>
-        <v>3.4833091436865082E-2</v>
+        <f t="shared" si="8"/>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="K24">
-        <f t="shared" ref="K24" si="14">ABS(K10-K$5)/(MAX(K$5:K$10)-MIN(K$5:K$10))</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
     </row>
@@ -1297,7 +1297,7 @@
       </c>
       <c r="C26">
         <f>MAX(C20,E20,G20,I20,K20)</f>
-        <v>0.63178294573643501</v>
+        <v>0.63200000000000001</v>
       </c>
       <c r="D26">
         <f>MAX(C26:C30)</f>
@@ -1311,24 +1311,24 @@
       </c>
       <c r="D27">
         <f>MIN(C26:C30)</f>
-        <v>0.53483309143686508</v>
+        <v>0.53500000000000003</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C28">
-        <f t="shared" ref="C28:C30" si="15">MAX(C22,E22,G22,I22,K22)</f>
-        <v>0.53483309143686508</v>
+        <f t="shared" ref="C28:C30" si="10">MAX(C22,E22,G22,I22,K22)</f>
+        <v>0.53500000000000003</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C29">
-        <f t="shared" si="15"/>
-        <v>0.73639896373057012</v>
+        <f t="shared" si="10"/>
+        <v>0.73650000000000004</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C30">
-        <f t="shared" si="15"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
     </row>
@@ -1337,64 +1337,70 @@
         <v>39</v>
       </c>
       <c r="C32">
-        <f>(C20*C$4)+(E20*E$4)+(G20*G$4)+(I20*I$4)+(K20*K$4)</f>
-        <v>0.3098723803429192</v>
+        <f>ROUND(((C20*C$4)+(E20*E$4)+(G20*G$4)+(I20*I$4)+(K20*K$4)), 4)</f>
+        <v>0.31</v>
       </c>
       <c r="D32">
         <f>MAX(C32:C36)</f>
-        <v>0.46822596547359918</v>
+        <v>0.46815000000000001</v>
       </c>
       <c r="F32">
-        <f>(((C32-$D$33)/($D$32-$D$33))*0.5)+(((C26-$D$27)/($D$26-$D$27))*0.5)</f>
-        <v>0.33526692864807028</v>
+        <f>ROUND(((((C32-$D$33)/($D$32-$D$33))*0.5)+(((C26-$D$27)/($D$26-$D$27))*0.5)), 3)</f>
+        <v>0.33600000000000002</v>
       </c>
     </row>
     <row r="33" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C33">
         <f>(C21*C$4)+(E21*E$4)+(G21*G$4)+(I21*I$4)+(K21*K$4)</f>
-        <v>0.21940632856955475</v>
+        <v>0.21935000000000004</v>
       </c>
       <c r="D33">
         <f>MIN(C32:C36)</f>
-        <v>0.17382586871501185</v>
+        <v>0.17380000000000001</v>
       </c>
       <c r="F33">
-        <f>(((C33-$D$33)/($D$32-$D$33))*0.5)+(((C27-$D$27)/($D$26-$D$27))*0.5)</f>
-        <v>0.57741244034291128</v>
+        <f t="shared" ref="F33:F36" si="11">ROUND(((((C33-$D$33)/($D$32-$D$33))*0.5)+(((C27-$D$27)/($D$26-$D$27))*0.5)), 3)</f>
+        <v>0.57699999999999996</v>
       </c>
     </row>
     <row r="34" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C34">
         <f>(C22*C$4)+(E22*E$4)+(G22*G$4)+(I22*I$4)+(K22*K$4)</f>
-        <v>0.37226033809711195</v>
+        <v>0.37229999999999996</v>
       </c>
       <c r="F34">
-        <f t="shared" ref="F34:F36" si="16">(((C34-$D$33)/($D$32-$D$33))*0.5)+(((C28-$D$27)/($D$26-$D$27))*0.5)</f>
-        <v>0.33701495272404658</v>
+        <f t="shared" si="11"/>
+        <v>0.33700000000000002</v>
       </c>
     </row>
     <row r="35" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C35">
         <f>(C23*C$4)+(E23*E$4)+(G23*G$4)+(I23*I$4)+(K23*K$4)</f>
-        <v>0.46822596547359918</v>
+        <v>0.46815000000000001</v>
       </c>
       <c r="F35">
-        <f t="shared" si="16"/>
-        <v>0.71665972856530857</v>
+        <f t="shared" si="11"/>
+        <v>0.71699999999999997</v>
       </c>
     </row>
     <row r="36" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C36">
         <f>(C24*C$4)+(E24*E$4)+(G24*G$4)+(I24*I$4)+(K24*K$4)</f>
-        <v>0.17382586871501185</v>
+        <v>0.17380000000000001</v>
       </c>
       <c r="F36">
-        <f t="shared" si="16"/>
+        <f t="shared" si="11"/>
         <v>0.5</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="J3:K3"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="F3:G3"/>
@@ -1404,12 +1410,6 @@
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="D3:E3"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="J3:K3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1485,26 +1485,26 @@
       <c r="A3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="16">
-        <v>3</v>
-      </c>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16">
-        <v>3</v>
-      </c>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16">
-        <v>2</v>
-      </c>
-      <c r="G3" s="16"/>
-      <c r="H3" s="15">
-        <v>2</v>
-      </c>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15">
-        <v>3</v>
-      </c>
-      <c r="K3" s="15"/>
+      <c r="B3" s="15">
+        <v>3</v>
+      </c>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15">
+        <v>3</v>
+      </c>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15">
+        <v>2</v>
+      </c>
+      <c r="G3" s="15"/>
+      <c r="H3" s="16">
+        <v>2</v>
+      </c>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16">
+        <v>3</v>
+      </c>
+      <c r="K3" s="16"/>
       <c r="P3" s="3" t="s">
         <v>26</v>
       </c>
@@ -2042,6 +2042,1230 @@
       <c r="F36" t="e">
         <f t="shared" si="10"/>
         <v>#DIV/0!</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="15">
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="J3:K3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="19.88671875" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" customWidth="1"/>
+    <col min="3" max="3" width="16.109375" customWidth="1"/>
+    <col min="4" max="4" width="17.5546875" customWidth="1"/>
+    <col min="5" max="6" width="17.88671875" customWidth="1"/>
+    <col min="7" max="7" width="17.5546875" customWidth="1"/>
+    <col min="8" max="9" width="17.77734375" customWidth="1"/>
+    <col min="10" max="10" width="17.44140625" customWidth="1"/>
+    <col min="11" max="11" width="17.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="15">
+        <v>2</v>
+      </c>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15">
+        <v>1</v>
+      </c>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15">
+        <v>4</v>
+      </c>
+      <c r="G3" s="15"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="9">
+        <v>0.3</v>
+      </c>
+      <c r="H4" s="2"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="9"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5">
+        <v>2.589</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5">
+        <v>2.3719999999999999</v>
+      </c>
+      <c r="F5" s="2"/>
+      <c r="G5">
+        <v>3.7730000000000001</v>
+      </c>
+      <c r="H5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="8"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="3">
+        <v>2</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" s="3">
+        <v>1</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" s="3">
+        <v>3</v>
+      </c>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="D8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8">
+        <v>3</v>
+      </c>
+      <c r="F8" t="s">
+        <v>46</v>
+      </c>
+      <c r="G8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C13" t="e">
+        <f>C5/C$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E13" t="e">
+        <f>E5/E$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G13" t="e">
+        <f>G5/G$11</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="3" t="e">
+        <f>C6/C$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" s="3" t="e">
+        <f>E6/E$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G14" s="3" t="e">
+        <f>G6/G$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="3" t="e">
+        <f t="shared" ref="C15:C18" si="0">C7/C$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="3" t="e">
+        <f t="shared" ref="E15:E18" si="1">E7/E$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F15" t="s">
+        <v>8</v>
+      </c>
+      <c r="G15" s="3" t="e">
+        <f t="shared" ref="G15:G18" si="2">G7/G$11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I15" s="3"/>
+      <c r="K15" s="3"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D16" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" s="3" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F16" t="s">
+        <v>6</v>
+      </c>
+      <c r="G16" s="3" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I16" s="3"/>
+      <c r="K16" s="3"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D17" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" s="3" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F17" t="s">
+        <v>24</v>
+      </c>
+      <c r="G17" s="3" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I17" s="3"/>
+      <c r="K17" s="3"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D18" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" s="3" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F18" t="s">
+        <v>6</v>
+      </c>
+      <c r="G18" s="3" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I18" s="3"/>
+      <c r="K18" s="3"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C20" s="12">
+        <f>ROUND((ABS(C6-C$5)/(MAX(C$5:C$10)-MIN(C$5:C$10))),4)</f>
+        <v>0.29449999999999998</v>
+      </c>
+      <c r="E20">
+        <f>ROUND((ABS(E6-E$5)/(MAX(E$5:E$10)-MIN(E$5:E$10))),4)</f>
+        <v>0.68600000000000005</v>
+      </c>
+      <c r="G20">
+        <f>ROUND((ABS(G6-G$5)/(MAX(G$5:G$10)-MIN(G$5:G$10))),4)</f>
+        <v>0.38650000000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C21" s="12">
+        <f t="shared" ref="C21:C22" si="3">ROUND((ABS(C7-C$5)/(MAX(C$5:C$10)-MIN(C$5:C$10))),4)</f>
+        <v>0.20549999999999999</v>
+      </c>
+      <c r="E21">
+        <f t="shared" ref="E21:E22" si="4">ROUND((ABS(E7-E$5)/(MAX(E$5:E$10)-MIN(E$5:E$10))),4)</f>
+        <v>0.186</v>
+      </c>
+      <c r="G21">
+        <f t="shared" ref="G21:G22" si="5">ROUND((ABS(G7-G$5)/(MAX(G$5:G$10)-MIN(G$5:G$10))),4)</f>
+        <v>0.1135</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C22" s="12">
+        <f t="shared" si="3"/>
+        <v>0.70550000000000002</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="4"/>
+        <v>0.314</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="5"/>
+        <v>0.61350000000000005</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B26" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C26">
+        <f>ROUND((MAX(C20,E20,G20,I20,K20)),4)</f>
+        <v>0.68600000000000005</v>
+      </c>
+      <c r="D26">
+        <f>MAX(C26:C30)</f>
+        <v>0.70550000000000002</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C27">
+        <f t="shared" ref="C27:C30" si="6">ROUND((MAX(C21,E21,G21,I21,K21)),4)</f>
+        <v>0.20549999999999999</v>
+      </c>
+      <c r="D27">
+        <f>MIN(C26:C30)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C28">
+        <f t="shared" si="6"/>
+        <v>0.70550000000000002</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C29">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C30">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B32" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C32">
+        <f>ROUND(((C20*C$4)+(E20*E$4)+(G20*G$4)+(I20*I$4)+(K20*K$4)),4)</f>
+        <v>0.51790000000000003</v>
+      </c>
+      <c r="D32">
+        <f>MAX(C32:C36)</f>
+        <v>0.51790000000000003</v>
+      </c>
+      <c r="F32">
+        <f>ROUND(((((C32-$D$33)/($D$32-$D$33))*0.5)+(((C26-$D$27)/($D$26-$D$27))*0.5)),4)</f>
+        <v>0.98619999999999997</v>
+      </c>
+    </row>
+    <row r="33" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C33">
+        <f t="shared" ref="C33:C36" si="7">ROUND(((C21*C$4)+(E21*E$4)+(G21*G$4)+(I21*I$4)+(K21*K$4)),4)</f>
+        <v>0.16819999999999999</v>
+      </c>
+      <c r="D33">
+        <f>MIN(C32:C36)</f>
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <f t="shared" ref="F33:F36" si="8">ROUND(((((C33-$D$33)/($D$32-$D$33))*0.5)+(((C27-$D$27)/($D$26-$D$27))*0.5)),4)</f>
+        <v>0.308</v>
+      </c>
+    </row>
+    <row r="34" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C34">
+        <f t="shared" si="7"/>
+        <v>0.48220000000000002</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="8"/>
+        <v>0.96550000000000002</v>
+      </c>
+    </row>
+    <row r="35" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C35">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C36">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="15">
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="J3:K3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K36"/>
+  <sheetViews>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32:F36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="19.109375" customWidth="1"/>
+    <col min="2" max="2" width="19.88671875" customWidth="1"/>
+    <col min="3" max="3" width="17.88671875" customWidth="1"/>
+    <col min="4" max="4" width="17.5546875" customWidth="1"/>
+    <col min="5" max="5" width="17.88671875" customWidth="1"/>
+    <col min="6" max="6" width="17.5546875" customWidth="1"/>
+    <col min="7" max="7" width="17.77734375" customWidth="1"/>
+    <col min="8" max="8" width="17.5546875" customWidth="1"/>
+    <col min="9" max="9" width="17.88671875" customWidth="1"/>
+    <col min="10" max="11" width="17.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="15">
+        <v>3</v>
+      </c>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15">
+        <v>3</v>
+      </c>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15">
+        <v>2</v>
+      </c>
+      <c r="G3" s="15"/>
+      <c r="H3" s="16">
+        <v>1</v>
+      </c>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="9">
+        <v>0.35</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="9">
+        <v>0.25</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="9">
+        <v>0.3</v>
+      </c>
+      <c r="H4" s="2"/>
+      <c r="I4" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="J4" s="2"/>
+      <c r="K4" s="9"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5">
+        <v>3.4089999999999998</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5">
+        <v>2.2639999999999998</v>
+      </c>
+      <c r="F5" s="2"/>
+      <c r="G5">
+        <v>2.5270000000000001</v>
+      </c>
+      <c r="H5" s="2"/>
+      <c r="I5">
+        <v>1.98</v>
+      </c>
+      <c r="J5" s="2"/>
+      <c r="K5" s="8"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="3">
+        <v>2</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="3">
+        <v>2</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" s="3">
+        <v>3</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I6" s="3">
+        <v>3</v>
+      </c>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+      <c r="F7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7">
+        <v>2</v>
+      </c>
+      <c r="H7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8" t="s">
+        <v>51</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8" t="s">
+        <v>46</v>
+      </c>
+      <c r="G8">
+        <v>5</v>
+      </c>
+      <c r="H8" t="s">
+        <v>21</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9">
+        <v>4</v>
+      </c>
+      <c r="D9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9">
+        <v>3</v>
+      </c>
+      <c r="F9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G9">
+        <v>3</v>
+      </c>
+      <c r="H9" t="s">
+        <v>9</v>
+      </c>
+      <c r="I9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="D10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
+      <c r="F10" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10">
+        <v>2</v>
+      </c>
+      <c r="H10" t="s">
+        <v>17</v>
+      </c>
+      <c r="I10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11">
+        <v>5</v>
+      </c>
+      <c r="E11">
+        <v>3</v>
+      </c>
+      <c r="G11">
+        <v>5</v>
+      </c>
+      <c r="I11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C13">
+        <f>C5/C$11</f>
+        <v>0.68179999999999996</v>
+      </c>
+      <c r="E13">
+        <f>E5/E$11</f>
+        <v>0.7546666666666666</v>
+      </c>
+      <c r="G13">
+        <f>G5/G$11</f>
+        <v>0.50540000000000007</v>
+      </c>
+      <c r="I13">
+        <f>I5/I$11</f>
+        <v>0.66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="3">
+        <f>C6/C$11</f>
+        <v>0.4</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" s="3">
+        <f>E6/E$11</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G14" s="3">
+        <f>G6/G$11</f>
+        <v>0.6</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I14" s="3">
+        <f>I6/I$11</f>
+        <v>1</v>
+      </c>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="3">
+        <f>C7/C$11</f>
+        <v>0.6</v>
+      </c>
+      <c r="D15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="3">
+        <f>E7/E$11</f>
+        <v>1</v>
+      </c>
+      <c r="F15" t="s">
+        <v>8</v>
+      </c>
+      <c r="G15" s="3">
+        <f>G7/G$11</f>
+        <v>0.4</v>
+      </c>
+      <c r="H15" t="s">
+        <v>17</v>
+      </c>
+      <c r="I15" s="3">
+        <f>I7/I$11</f>
+        <v>1</v>
+      </c>
+      <c r="K15" s="3"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="3">
+        <f>C8/C$11</f>
+        <v>0.4</v>
+      </c>
+      <c r="D16" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" s="3">
+        <f>E8/E$11</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F16" t="s">
+        <v>6</v>
+      </c>
+      <c r="G16" s="3">
+        <f>G8/G$11</f>
+        <v>1</v>
+      </c>
+      <c r="H16" t="s">
+        <v>21</v>
+      </c>
+      <c r="I16" s="3">
+        <f>I8/I$11</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="K16" s="3"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="3">
+        <f>C9/C$11</f>
+        <v>0.8</v>
+      </c>
+      <c r="D17" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" s="3">
+        <f>E9/E$11</f>
+        <v>1</v>
+      </c>
+      <c r="F17" t="s">
+        <v>24</v>
+      </c>
+      <c r="G17" s="3">
+        <f>G9/G$11</f>
+        <v>0.6</v>
+      </c>
+      <c r="H17" t="s">
+        <v>23</v>
+      </c>
+      <c r="I17" s="3">
+        <f>I9/I$11</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="K17" s="3"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="3" t="e">
+        <f>#REF!/C$11</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D18" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" s="3" t="e">
+        <f>#REF!/E$11</f>
+        <v>#REF!</v>
+      </c>
+      <c r="F18" t="s">
+        <v>6</v>
+      </c>
+      <c r="G18" s="3" t="e">
+        <f>#REF!/G$11</f>
+        <v>#REF!</v>
+      </c>
+      <c r="H18" t="s">
+        <v>9</v>
+      </c>
+      <c r="I18" s="3" t="e">
+        <f>#REF!/I$11</f>
+        <v>#REF!</v>
+      </c>
+      <c r="K18" s="3"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C20">
+        <f>ROUND((ABS(C6-C$5)/(MAX(C$5:C$10)-MIN(C$5:C$10))), 4)</f>
+        <v>0.70450000000000002</v>
+      </c>
+      <c r="E20">
+        <f xml:space="preserve"> ROUND((ABS(E6-E$5)/(MAX(E$5:E$10)-MIN(E$5:E$10))),4)</f>
+        <v>0.13200000000000001</v>
+      </c>
+      <c r="G20">
+        <f>ROUND((ABS(G6-G$5)/(MAX(G$5:G$10)-MIN(G$5:G$10))),4)</f>
+        <v>0.15770000000000001</v>
+      </c>
+      <c r="I20">
+        <f>ROUND((ABS(I6-I$5)/(MAX(I$5:I$10)-MIN(I$5:I$10))),4)</f>
+        <v>0.51</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C21">
+        <f t="shared" ref="C21:C24" si="0">ROUND((ABS(C7-C$5)/(MAX(C$5:C$10)-MIN(C$5:C$10))), 4)</f>
+        <v>0.20449999999999999</v>
+      </c>
+      <c r="E21">
+        <f t="shared" ref="E21:E24" si="1" xml:space="preserve"> ROUND((ABS(E7-E$5)/(MAX(E$5:E$10)-MIN(E$5:E$10))),4)</f>
+        <v>0.36799999999999999</v>
+      </c>
+      <c r="G21">
+        <f t="shared" ref="G21:G24" si="2">ROUND((ABS(G7-G$5)/(MAX(G$5:G$10)-MIN(G$5:G$10))),4)</f>
+        <v>0.1757</v>
+      </c>
+      <c r="I21">
+        <f t="shared" ref="I21:I24" si="3">ROUND((ABS(I7-I$5)/(MAX(I$5:I$10)-MIN(I$5:I$10))),4)</f>
+        <v>0.51</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C22">
+        <f t="shared" si="0"/>
+        <v>0.70450000000000002</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="1"/>
+        <v>0.63200000000000001</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="2"/>
+        <v>0.82430000000000003</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="3"/>
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C23">
+        <f t="shared" si="0"/>
+        <v>0.29549999999999998</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="1"/>
+        <v>0.36799999999999999</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="2"/>
+        <v>0.15770000000000001</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="3"/>
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C24">
+        <f t="shared" si="0"/>
+        <v>0.20449999999999999</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="1"/>
+        <v>0.13200000000000001</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="2"/>
+        <v>0.1757</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="3"/>
+        <v>0.51</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B26" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C26">
+        <f>ROUND((MAX(C20,E20,G20,I20,K20)),4)</f>
+        <v>0.70450000000000002</v>
+      </c>
+      <c r="D26">
+        <f>MAX(C26:C30)</f>
+        <v>0.82430000000000003</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C27">
+        <f t="shared" ref="C27:C30" si="4">ROUND((MAX(C21,E21,G21,I21,K21)),4)</f>
+        <v>0.51</v>
+      </c>
+      <c r="D27">
+        <f>MIN(C26:C30)</f>
+        <v>0.36799999999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C28">
+        <f t="shared" si="4"/>
+        <v>0.82430000000000003</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C29">
+        <f t="shared" si="4"/>
+        <v>0.36799999999999999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C30">
+        <f t="shared" si="4"/>
+        <v>0.51</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B32" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C32">
+        <f>ROUND(((C20*C$4)+(E20*E$4)+(G20*G$4)+(I20*I$4)+(K20*K$4)),4)</f>
+        <v>0.37790000000000001</v>
+      </c>
+      <c r="D32">
+        <f>MAX(C32:C36)</f>
+        <v>0.70089999999999997</v>
+      </c>
+      <c r="F32">
+        <f>ROUND(((((C32-$D$33)/($D$32-$D$33))*0.5)+(((C26-$D$27)/($D$26-$D$27))*0.5)),4)</f>
+        <v>0.54090000000000005</v>
+      </c>
+    </row>
+    <row r="33" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C33">
+        <f t="shared" ref="C33:C36" si="5">ROUND(((C21*C$4)+(E21*E$4)+(G21*G$4)+(I21*I$4)+(K21*K$4)),4)</f>
+        <v>0.26729999999999998</v>
+      </c>
+      <c r="D33">
+        <f>MIN(C32:C36)</f>
+        <v>0.20830000000000001</v>
+      </c>
+      <c r="F33">
+        <f t="shared" ref="F33:F36" si="6">ROUND(((((C33-$D$33)/($D$32-$D$33))*0.5)+(((C27-$D$27)/($D$26-$D$27))*0.5)),4)</f>
+        <v>0.2155</v>
+      </c>
+    </row>
+    <row r="34" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C34">
+        <f t="shared" si="5"/>
+        <v>0.70089999999999997</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C35">
+        <f t="shared" si="5"/>
+        <v>0.2437</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="6"/>
+        <v>3.5900000000000001E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C36">
+        <f t="shared" si="5"/>
+        <v>0.20830000000000001</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="6"/>
+        <v>0.15559999999999999</v>
       </c>
     </row>
   </sheetData>
@@ -2067,1236 +3291,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K36"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F32" sqref="F32:F34"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="19.88671875" customWidth="1"/>
-    <col min="2" max="2" width="16.33203125" customWidth="1"/>
-    <col min="3" max="3" width="16.109375" customWidth="1"/>
-    <col min="4" max="4" width="17.5546875" customWidth="1"/>
-    <col min="5" max="6" width="17.88671875" customWidth="1"/>
-    <col min="7" max="7" width="17.5546875" customWidth="1"/>
-    <col min="8" max="9" width="17.77734375" customWidth="1"/>
-    <col min="10" max="10" width="17.44140625" customWidth="1"/>
-    <col min="11" max="11" width="17.88671875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B1" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" s="16">
-        <v>2</v>
-      </c>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16">
-        <v>1</v>
-      </c>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16">
-        <v>4</v>
-      </c>
-      <c r="G3" s="16"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15"/>
-      <c r="K3" s="15"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="F4" s="2"/>
-      <c r="G4" s="9">
-        <v>0.3</v>
-      </c>
-      <c r="H4" s="2"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="9"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B5" s="2"/>
-      <c r="C5">
-        <v>2.5889443059019133</v>
-      </c>
-      <c r="D5" s="2"/>
-      <c r="E5">
-        <v>2.3720930232558133</v>
-      </c>
-      <c r="F5" s="2"/>
-      <c r="G5">
-        <v>3.7733160621761663</v>
-      </c>
-      <c r="H5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="8"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="3">
-        <v>2</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E6" s="3">
-        <v>1</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G6" s="3">
-        <v>3</v>
-      </c>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="B7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7">
-        <v>3</v>
-      </c>
-      <c r="D7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7">
-        <v>2</v>
-      </c>
-      <c r="F7" t="s">
-        <v>24</v>
-      </c>
-      <c r="G7">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="B8" t="s">
-        <v>45</v>
-      </c>
-      <c r="C8">
-        <v>4</v>
-      </c>
-      <c r="D8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8">
-        <v>3</v>
-      </c>
-      <c r="F8" t="s">
-        <v>46</v>
-      </c>
-      <c r="G8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C13" t="e">
-        <f>C5/C$11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E13" t="e">
-        <f>E5/E$11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G13" t="e">
-        <f>G5/G$11</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14" s="3" t="e">
-        <f>C6/C$11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E14" s="3" t="e">
-        <f>E6/E$11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G14" s="3" t="e">
-        <f>G6/G$11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" s="3" t="e">
-        <f t="shared" ref="C15:C18" si="0">C7/C$11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D15" t="s">
-        <v>13</v>
-      </c>
-      <c r="E15" s="3" t="e">
-        <f t="shared" ref="E15:E18" si="1">E7/E$11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F15" t="s">
-        <v>8</v>
-      </c>
-      <c r="G15" s="3" t="e">
-        <f t="shared" ref="G15:G18" si="2">G7/G$11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I15" s="3"/>
-      <c r="K15" s="3"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16" t="s">
-        <v>20</v>
-      </c>
-      <c r="C16" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D16" t="s">
-        <v>7</v>
-      </c>
-      <c r="E16" s="3" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F16" t="s">
-        <v>6</v>
-      </c>
-      <c r="G16" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I16" s="3"/>
-      <c r="K16" s="3"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>22</v>
-      </c>
-      <c r="B17" t="s">
-        <v>12</v>
-      </c>
-      <c r="C17" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D17" t="s">
-        <v>7</v>
-      </c>
-      <c r="E17" s="3" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F17" t="s">
-        <v>24</v>
-      </c>
-      <c r="G17" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I17" s="3"/>
-      <c r="K17" s="3"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>26</v>
-      </c>
-      <c r="B18" t="s">
-        <v>6</v>
-      </c>
-      <c r="C18" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D18" t="s">
-        <v>7</v>
-      </c>
-      <c r="E18" s="3" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F18" t="s">
-        <v>6</v>
-      </c>
-      <c r="G18" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I18" s="3"/>
-      <c r="K18" s="3"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C20" s="12">
-        <f>ABS(C6-C$5)/(MAX(C$5:C$10)-MIN(C$5:C$10))</f>
-        <v>0.29447215295095663</v>
-      </c>
-      <c r="E20">
-        <f>ABS(E6-E$5)/(MAX(E$5:E$10)-MIN(E$5:E$10))</f>
-        <v>0.68604651162790664</v>
-      </c>
-      <c r="G20">
-        <f>ABS(G6-G$5)/(MAX(G$5:G$10)-MIN(G$5:G$10))</f>
-        <v>0.38665803108808317</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C21">
-        <f t="shared" ref="C21:E22" si="3">ABS(C7-C$5)/(MAX(C$5:C$10)-MIN(C$5:C$10))</f>
-        <v>0.20552784704904337</v>
-      </c>
-      <c r="E21">
-        <f t="shared" si="3"/>
-        <v>0.18604651162790664</v>
-      </c>
-      <c r="G21">
-        <f t="shared" ref="G21:G22" si="4">ABS(G7-G$5)/(MAX(G$5:G$10)-MIN(G$5:G$10))</f>
-        <v>0.11334196891191683</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C22">
-        <f t="shared" si="3"/>
-        <v>0.70552784704904337</v>
-      </c>
-      <c r="E22">
-        <f t="shared" si="3"/>
-        <v>0.31395348837209336</v>
-      </c>
-      <c r="G22">
-        <f t="shared" si="4"/>
-        <v>0.61334196891191683</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B26" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="C26">
-        <f>MAX(C20,E20,G20,I20,K20)</f>
-        <v>0.68604651162790664</v>
-      </c>
-      <c r="D26">
-        <f>MAX(C26:C30)</f>
-        <v>0.70552784704904337</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C27">
-        <f>MAX(C21,E21,G21,I21,K21)</f>
-        <v>0.20552784704904337</v>
-      </c>
-      <c r="D27">
-        <f>MIN(C26:C30)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C28">
-        <f t="shared" ref="C28:C30" si="5">MAX(C22,E22,G22,I22,K22)</f>
-        <v>0.70552784704904337</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C29">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C30">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B32" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C32">
-        <f>(C20*C$4)+(E20*E$4)+(G20*G$4)+(I20*I$4)+(K20*K$4)</f>
-        <v>0.5179150957305696</v>
-      </c>
-      <c r="D32">
-        <f>MAX(C32:C36)</f>
-        <v>0.5179150957305696</v>
-      </c>
-      <c r="F32">
-        <f>(((C32-$D$33)/($D$32-$D$33))*0.5)+(((C26-$D$27)/($D$26-$D$27))*0.5)</f>
-        <v>0.9861937870329146</v>
-      </c>
-    </row>
-    <row r="33" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C33">
-        <f>(C21*C$4)+(E21*E$4)+(G21*G$4)+(I21*I$4)+(K21*K$4)</f>
-        <v>0.16813141589733704</v>
-      </c>
-      <c r="D33">
-        <f>MIN(C32:C36)</f>
-        <v>0</v>
-      </c>
-      <c r="F33">
-        <f>(((C33-$D$33)/($D$32-$D$33))*0.5)+(((C27-$D$27)/($D$26-$D$27))*0.5)</f>
-        <v>0.30797099184086668</v>
-      </c>
-    </row>
-    <row r="34" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C34">
-        <f>(C22*C$4)+(E22*E$4)+(G22*G$4)+(I22*I$4)+(K22*K$4)</f>
-        <v>0.4820849042694304</v>
-      </c>
-      <c r="F34">
-        <f t="shared" ref="F34:F36" si="6">(((C34-$D$33)/($D$32-$D$33))*0.5)+(((C28-$D$27)/($D$26-$D$27))*0.5)</f>
-        <v>0.96540920340369962</v>
-      </c>
-    </row>
-    <row r="35" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C35">
-        <f>(C23*C$4)+(E23*E$4)+(G23*G$4)+(I23*I$4)+(K23*K$4)</f>
-        <v>0</v>
-      </c>
-      <c r="F35">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C36">
-        <f>(C24*C$4)+(E24*E$4)+(G24*G$4)+(I24*I$4)+(K24*K$4)</f>
-        <v>0</v>
-      </c>
-      <c r="F36">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:K2"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K36"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="19.109375" customWidth="1"/>
-    <col min="2" max="2" width="19.88671875" customWidth="1"/>
-    <col min="3" max="3" width="17.88671875" customWidth="1"/>
-    <col min="4" max="4" width="17.5546875" customWidth="1"/>
-    <col min="5" max="5" width="17.88671875" customWidth="1"/>
-    <col min="6" max="6" width="17.5546875" customWidth="1"/>
-    <col min="7" max="7" width="17.77734375" customWidth="1"/>
-    <col min="8" max="8" width="17.5546875" customWidth="1"/>
-    <col min="9" max="9" width="17.88671875" customWidth="1"/>
-    <col min="10" max="11" width="17.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B1" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" s="16">
-        <v>3</v>
-      </c>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16">
-        <v>3</v>
-      </c>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16">
-        <v>2</v>
-      </c>
-      <c r="G3" s="16"/>
-      <c r="H3" s="15">
-        <v>1</v>
-      </c>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15"/>
-      <c r="K3" s="15"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="9">
-        <v>0.35</v>
-      </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="9">
-        <v>0.25</v>
-      </c>
-      <c r="F4" s="2"/>
-      <c r="G4" s="9">
-        <v>0.3</v>
-      </c>
-      <c r="H4" s="2"/>
-      <c r="I4" s="9">
-        <v>0.1</v>
-      </c>
-      <c r="J4" s="2"/>
-      <c r="K4" s="9"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B5" s="2"/>
-      <c r="C5">
-        <v>3.4093931837073996</v>
-      </c>
-      <c r="D5" s="2"/>
-      <c r="E5">
-        <v>2.26356589147287</v>
-      </c>
-      <c r="F5" s="2"/>
-      <c r="G5">
-        <v>2.5272020725388598</v>
-      </c>
-      <c r="H5" s="2"/>
-      <c r="I5">
-        <v>1.9796806966618299</v>
-      </c>
-      <c r="J5" s="2"/>
-      <c r="K5" s="8"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="3">
-        <v>2</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="3">
-        <v>2</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G6" s="3">
-        <v>3</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="I6" s="3">
-        <v>3</v>
-      </c>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="B7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7">
-        <v>3</v>
-      </c>
-      <c r="D7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7">
-        <v>3</v>
-      </c>
-      <c r="F7" t="s">
-        <v>8</v>
-      </c>
-      <c r="G7">
-        <v>2</v>
-      </c>
-      <c r="H7" t="s">
-        <v>17</v>
-      </c>
-      <c r="I7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="B8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8">
-        <v>2</v>
-      </c>
-      <c r="D8" t="s">
-        <v>51</v>
-      </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-      <c r="F8" t="s">
-        <v>46</v>
-      </c>
-      <c r="G8">
-        <v>5</v>
-      </c>
-      <c r="H8" t="s">
-        <v>21</v>
-      </c>
-      <c r="I8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="B9" t="s">
-        <v>45</v>
-      </c>
-      <c r="C9">
-        <v>4</v>
-      </c>
-      <c r="D9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9">
-        <v>3</v>
-      </c>
-      <c r="F9" t="s">
-        <v>6</v>
-      </c>
-      <c r="G9">
-        <v>3</v>
-      </c>
-      <c r="H9" t="s">
-        <v>9</v>
-      </c>
-      <c r="I9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10">
-        <v>3</v>
-      </c>
-      <c r="D10" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10">
-        <v>2</v>
-      </c>
-      <c r="F10" t="s">
-        <v>8</v>
-      </c>
-      <c r="G10">
-        <v>2</v>
-      </c>
-      <c r="H10" t="s">
-        <v>17</v>
-      </c>
-      <c r="I10">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C11">
-        <v>5</v>
-      </c>
-      <c r="E11">
-        <v>3</v>
-      </c>
-      <c r="G11">
-        <v>5</v>
-      </c>
-      <c r="I11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C13">
-        <f>C5/C$11</f>
-        <v>0.68187863674147997</v>
-      </c>
-      <c r="E13">
-        <f>E5/E$11</f>
-        <v>0.75452196382429004</v>
-      </c>
-      <c r="G13">
-        <f>G5/G$11</f>
-        <v>0.505440414507772</v>
-      </c>
-      <c r="I13">
-        <f>I5/I$11</f>
-        <v>0.6598935655539433</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14" s="3">
-        <f>C6/C$11</f>
-        <v>0.4</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E14" s="3">
-        <f>E6/E$11</f>
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G14" s="3">
-        <f>G6/G$11</f>
-        <v>0.6</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I14" s="3">
-        <f>I6/I$11</f>
-        <v>1</v>
-      </c>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" s="3">
-        <f>C7/C$11</f>
-        <v>0.6</v>
-      </c>
-      <c r="D15" t="s">
-        <v>13</v>
-      </c>
-      <c r="E15" s="3">
-        <f>E7/E$11</f>
-        <v>1</v>
-      </c>
-      <c r="F15" t="s">
-        <v>8</v>
-      </c>
-      <c r="G15" s="3">
-        <f>G7/G$11</f>
-        <v>0.4</v>
-      </c>
-      <c r="H15" t="s">
-        <v>17</v>
-      </c>
-      <c r="I15" s="3">
-        <f>I7/I$11</f>
-        <v>1</v>
-      </c>
-      <c r="K15" s="3"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16" t="s">
-        <v>20</v>
-      </c>
-      <c r="C16" s="3">
-        <f>C8/C$11</f>
-        <v>0.4</v>
-      </c>
-      <c r="D16" t="s">
-        <v>7</v>
-      </c>
-      <c r="E16" s="3">
-        <f>E8/E$11</f>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="F16" t="s">
-        <v>6</v>
-      </c>
-      <c r="G16" s="3">
-        <f>G8/G$11</f>
-        <v>1</v>
-      </c>
-      <c r="H16" t="s">
-        <v>21</v>
-      </c>
-      <c r="I16" s="3">
-        <f>I8/I$11</f>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="K16" s="3"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>22</v>
-      </c>
-      <c r="B17" t="s">
-        <v>12</v>
-      </c>
-      <c r="C17" s="3">
-        <f>C9/C$11</f>
-        <v>0.8</v>
-      </c>
-      <c r="D17" t="s">
-        <v>7</v>
-      </c>
-      <c r="E17" s="3">
-        <f>E9/E$11</f>
-        <v>1</v>
-      </c>
-      <c r="F17" t="s">
-        <v>24</v>
-      </c>
-      <c r="G17" s="3">
-        <f>G9/G$11</f>
-        <v>0.6</v>
-      </c>
-      <c r="H17" t="s">
-        <v>23</v>
-      </c>
-      <c r="I17" s="3">
-        <f>I9/I$11</f>
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="K17" s="3"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>26</v>
-      </c>
-      <c r="B18" t="s">
-        <v>6</v>
-      </c>
-      <c r="C18" s="3" t="e">
-        <f>#REF!/C$11</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D18" t="s">
-        <v>7</v>
-      </c>
-      <c r="E18" s="3" t="e">
-        <f>#REF!/E$11</f>
-        <v>#REF!</v>
-      </c>
-      <c r="F18" t="s">
-        <v>6</v>
-      </c>
-      <c r="G18" s="3" t="e">
-        <f>#REF!/G$11</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H18" t="s">
-        <v>9</v>
-      </c>
-      <c r="I18" s="3" t="e">
-        <f>#REF!/I$11</f>
-        <v>#REF!</v>
-      </c>
-      <c r="K18" s="3"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C20">
-        <f>ABS(C6-C$5)/(MAX(C$5:C$10)-MIN(C$5:C$10))</f>
-        <v>0.70469659185369982</v>
-      </c>
-      <c r="E20">
-        <f>ABS(E6-E$5)/(MAX(E$5:E$10)-MIN(E$5:E$10))</f>
-        <v>0.13178294573643501</v>
-      </c>
-      <c r="G20">
-        <f>ABS(G6-G$5)/(MAX(G$5:G$10)-MIN(G$5:G$10))</f>
-        <v>0.15759930915371342</v>
-      </c>
-      <c r="I20">
-        <f>ABS(I6-I$5)/(MAX(I$5:I$10)-MIN(I$5:I$10))</f>
-        <v>0.51015965166908506</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C21">
-        <f>ABS(C7-C$5)/(MAX(C$5:C$10)-MIN(C$5:C$10))</f>
-        <v>0.20469659185369982</v>
-      </c>
-      <c r="E21">
-        <f>ABS(E7-E$5)/(MAX(E$5:E$10)-MIN(E$5:E$10))</f>
-        <v>0.36821705426356499</v>
-      </c>
-      <c r="G21">
-        <f>ABS(G7-G$5)/(MAX(G$5:G$10)-MIN(G$5:G$10))</f>
-        <v>0.17573402417961992</v>
-      </c>
-      <c r="I21">
-        <f>ABS(I7-I$5)/(MAX(I$5:I$10)-MIN(I$5:I$10))</f>
-        <v>0.51015965166908506</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C22">
-        <f>ABS(C8-C$5)/(MAX(C$5:C$10)-MIN(C$5:C$10))</f>
-        <v>0.70469659185369982</v>
-      </c>
-      <c r="E22">
-        <f>ABS(E8-E$5)/(MAX(E$5:E$10)-MIN(E$5:E$10))</f>
-        <v>0.63178294573643501</v>
-      </c>
-      <c r="G22">
-        <f>ABS(G8-G$5)/(MAX(G$5:G$10)-MIN(G$5:G$10))</f>
-        <v>0.82426597582038008</v>
-      </c>
-      <c r="I22">
-        <f>ABS(I8-I$5)/(MAX(I$5:I$10)-MIN(I$5:I$10))</f>
-        <v>0.48984034833091494</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C23">
-        <f>ABS(C9-C$5)/(MAX(C$5:C$10)-MIN(C$5:C$10))</f>
-        <v>0.29530340814630018</v>
-      </c>
-      <c r="E23">
-        <f>ABS(E9-E$5)/(MAX(E$5:E$10)-MIN(E$5:E$10))</f>
-        <v>0.36821705426356499</v>
-      </c>
-      <c r="G23">
-        <f>ABS(G9-G$5)/(MAX(G$5:G$10)-MIN(G$5:G$10))</f>
-        <v>0.15759930915371342</v>
-      </c>
-      <c r="I23">
-        <f>ABS(I9-I$5)/(MAX(I$5:I$10)-MIN(I$5:I$10))</f>
-        <v>1.0159651669085057E-2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C24">
-        <f>ABS(C10-C$5)/(MAX(C$5:C$10)-MIN(C$5:C$10))</f>
-        <v>0.20469659185369982</v>
-      </c>
-      <c r="E24">
-        <f>ABS(E10-E$5)/(MAX(E$5:E$10)-MIN(E$5:E$10))</f>
-        <v>0.13178294573643501</v>
-      </c>
-      <c r="G24">
-        <f>ABS(G10-G$5)/(MAX(G$5:G$10)-MIN(G$5:G$10))</f>
-        <v>0.17573402417961992</v>
-      </c>
-      <c r="I24">
-        <f>ABS(I10-I$5)/(MAX(I$5:I$10)-MIN(I$5:I$10))</f>
-        <v>0.51015965166908506</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B26" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="C26">
-        <f>MAX(C20,E20,G20,I20,K20)</f>
-        <v>0.70469659185369982</v>
-      </c>
-      <c r="D26">
-        <f>MAX(C26:C30)</f>
-        <v>0.82426597582038008</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C27">
-        <f>MAX(C21,E21,G21,I21,K21)</f>
-        <v>0.51015965166908506</v>
-      </c>
-      <c r="D27">
-        <f>MIN(C26:C30)</f>
-        <v>0.36821705426356499</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C28">
-        <f t="shared" ref="C28:C30" si="0">MAX(C22,E22,G22,I22,K22)</f>
-        <v>0.82426597582038008</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C29">
-        <f t="shared" si="0"/>
-        <v>0.36821705426356499</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C30">
-        <f t="shared" si="0"/>
-        <v>0.51015965166908506</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B32" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C32">
-        <f>(C20*C$4)+(E20*E$4)+(G20*G$4)+(I20*I$4)+(K20*K$4)</f>
-        <v>0.37788530149592625</v>
-      </c>
-      <c r="D32">
-        <f>MAX(C32:C36)</f>
-        <v>0.70085337116210922</v>
-      </c>
-      <c r="F32">
-        <f>(((C32-$D$33)/($D$32-$D$33))*0.5)+(((C26-$D$27)/($D$26-$D$27))*0.5)</f>
-        <v>0.54103932899766782</v>
-      </c>
-    </row>
-    <row r="33" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C33">
-        <f>(C21*C$4)+(E21*E$4)+(G21*G$4)+(I21*I$4)+(K21*K$4)</f>
-        <v>0.2674342431354807</v>
-      </c>
-      <c r="D33">
-        <f>MIN(C32:C36)</f>
-        <v>0.20832571600369817</v>
-      </c>
-      <c r="F33">
-        <f>(((C33-$D$33)/($D$32-$D$33))*0.5)+(((C27-$D$27)/($D$26-$D$27))*0.5)</f>
-        <v>0.2156274046967247</v>
-      </c>
-    </row>
-    <row r="34" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C34">
-        <f>(C22*C$4)+(E22*E$4)+(G22*G$4)+(I22*I$4)+(K22*K$4)</f>
-        <v>0.70085337116210922</v>
-      </c>
-      <c r="F34">
-        <f t="shared" ref="F34:F36" si="1">(((C34-$D$33)/($D$32-$D$33))*0.5)+(((C28-$D$27)/($D$26-$D$27))*0.5)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C35">
-        <f>(C23*C$4)+(E23*E$4)+(G23*G$4)+(I23*I$4)+(K23*K$4)</f>
-        <v>0.24370621433011883</v>
-      </c>
-      <c r="F35">
-        <f t="shared" si="1"/>
-        <v>3.5917270792683982E-2</v>
-      </c>
-    </row>
-    <row r="36" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C36">
-        <f>(C24*C$4)+(E24*E$4)+(G24*G$4)+(I24*I$4)+(K24*K$4)</f>
-        <v>0.20832571600369817</v>
-      </c>
-      <c r="F36">
-        <f t="shared" si="1"/>
-        <v>0.15562211716340688</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="J3:K3"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="W22" sqref="W22"/>
+      <selection activeCell="Q25" sqref="Q25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4259,8 +4259,8 @@
         <v>4</v>
       </c>
       <c r="E22">
-        <f>(B22+C22+D22)/3</f>
-        <v>2.4351620947630934</v>
+        <f>ROUND(((B22+C22+D22)/3), 3)</f>
+        <v>2.4350000000000001</v>
       </c>
       <c r="H22">
         <v>2</v>
@@ -4272,8 +4272,8 @@
         <v>3</v>
       </c>
       <c r="K22">
-        <f>(H22+I22+J22)/3</f>
-        <v>2.3720930232558133</v>
+        <f>ROUND(((H22+I22+J22)/3), 3)</f>
+        <v>2.3719999999999999</v>
       </c>
       <c r="N22">
         <v>1</v>
@@ -4285,8 +4285,8 @@
         <v>3</v>
       </c>
       <c r="Q22">
-        <f>(N22+O22+P22)/3</f>
-        <v>2.0708117443868734</v>
+        <f>ROUND(((N22+O22+P22)/3), 3)</f>
+        <v>2.0710000000000002</v>
       </c>
       <c r="T22">
         <v>1</v>
@@ -4298,8 +4298,8 @@
         <v>3</v>
       </c>
       <c r="W22">
-        <f>(T22+U22+V22)/3</f>
-        <v>1.9796806966618299</v>
+        <f>ROUND(((T22+U22+V22)/3), 3)</f>
+        <v>1.98</v>
       </c>
       <c r="Z22">
         <v>1</v>
@@ -4311,8 +4311,8 @@
         <v>3</v>
       </c>
       <c r="AC22">
-        <f>(Z22+AA22+AB22)/3</f>
-        <v>1.9185750636132299</v>
+        <f>ROUND(((Z22+AA22+AB22)/3), 3)</f>
+        <v>1.919</v>
       </c>
     </row>
     <row r="23" spans="1:29" x14ac:dyDescent="0.3">
@@ -4326,8 +4326,8 @@
         <v>4</v>
       </c>
       <c r="E23">
-        <f t="shared" ref="E23:E26" si="5">(B23+C23+D23)/3</f>
-        <v>2.5889443059019133</v>
+        <f t="shared" ref="E23:E26" si="5">ROUND(((B23+C23+D23)/3), 3)</f>
+        <v>2.589</v>
       </c>
       <c r="H23">
         <v>2</v>
@@ -4339,8 +4339,8 @@
         <v>3</v>
       </c>
       <c r="K23">
-        <f t="shared" ref="K23:K24" si="6">(H23+I23+J23)/3</f>
-        <v>2.4844961240310064</v>
+        <f t="shared" ref="K23:K24" si="6">ROUND(((H23+I23+J23)/3), 3)</f>
+        <v>2.484</v>
       </c>
       <c r="N23">
         <v>1</v>
@@ -4352,8 +4352,8 @@
         <v>4</v>
       </c>
       <c r="Q23">
-        <f t="shared" ref="Q23:Q26" si="7">(N23+O23+P23)/3</f>
-        <v>2.5272020725388598</v>
+        <f t="shared" ref="Q23:Q26" si="7">ROUND(((N23+O23+P23)/3), 3)</f>
+        <v>2.5270000000000001</v>
       </c>
       <c r="T23">
         <v>1</v>
@@ -4365,8 +4365,8 @@
         <v>3</v>
       </c>
       <c r="W23">
-        <f t="shared" ref="W23:W24" si="8">(T23+U23+V23)/3</f>
-        <v>2.0696661828737302</v>
+        <f t="shared" ref="W23:W24" si="8">ROUND(((T23+U23+V23)/3), 3)</f>
+        <v>2.0699999999999998</v>
       </c>
       <c r="Z23">
         <v>2</v>
@@ -4378,8 +4378,8 @@
         <v>3</v>
       </c>
       <c r="AC23">
-        <f t="shared" ref="AC23:AC24" si="9">(Z23+AA23+AB23)/3</f>
-        <v>2.3727735368956733</v>
+        <f t="shared" ref="AC23:AC24" si="9">ROUND(((Z23+AA23+AB23)/3), 3)</f>
+        <v>2.3730000000000002</v>
       </c>
     </row>
     <row r="24" spans="1:29" x14ac:dyDescent="0.3">
@@ -4394,7 +4394,7 @@
       </c>
       <c r="E24">
         <f t="shared" si="5"/>
-        <v>3.4093931837073996</v>
+        <v>3.4089999999999998</v>
       </c>
       <c r="H24">
         <v>1</v>
@@ -4407,7 +4407,7 @@
       </c>
       <c r="K24">
         <f t="shared" si="6"/>
-        <v>2.26356589147287</v>
+        <v>2.2639999999999998</v>
       </c>
       <c r="N24">
         <v>2</v>
@@ -4420,7 +4420,7 @@
       </c>
       <c r="Q24">
         <f t="shared" si="7"/>
-        <v>2.983592400690847</v>
+        <v>2.984</v>
       </c>
       <c r="T24">
         <v>1</v>
@@ -4433,7 +4433,7 @@
       </c>
       <c r="W24">
         <f t="shared" si="8"/>
-        <v>2.1596516690856302</v>
+        <v>2.16</v>
       </c>
       <c r="Z24">
         <v>1</v>
@@ -4446,7 +4446,7 @@
       </c>
       <c r="AC24">
         <f t="shared" si="9"/>
-        <v>2.1603053435114501</v>
+        <v>2.16</v>
       </c>
     </row>
     <row r="25" spans="1:29" x14ac:dyDescent="0.3">
@@ -4461,7 +4461,7 @@
       </c>
       <c r="E25">
         <f t="shared" si="5"/>
-        <v>3.5631753948462168</v>
+        <v>3.5630000000000002</v>
       </c>
       <c r="N25">
         <v>3</v>
@@ -4474,7 +4474,7 @@
       </c>
       <c r="Q25">
         <f t="shared" si="7"/>
-        <v>3.7733160621761663</v>
+        <v>3.7730000000000001</v>
       </c>
     </row>
     <row r="26" spans="1:29" x14ac:dyDescent="0.3">
@@ -4489,7 +4489,7 @@
       </c>
       <c r="E26">
         <f t="shared" si="5"/>
-        <v>3.7169576059850371</v>
+        <v>3.7170000000000001</v>
       </c>
       <c r="N26">
         <v>2</v>
@@ -4502,7 +4502,7 @@
       </c>
       <c r="Q26">
         <f t="shared" si="7"/>
-        <v>3.2297063903281535</v>
+        <v>3.23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>